<commit_message>
Updating table definition spreadsheet
</commit_message>
<xml_diff>
--- a/TableCrossReference.xlsx
+++ b/TableCrossReference.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ljr\git\genTeamsStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA13385-FE46-48D2-918B-335799273BA4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137BF3E9-4A51-46C8-82EE-D948E04AF39C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{783EAF43-63E2-4C6E-A04D-4784F852E72D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{783EAF43-63E2-4C6E-A04D-4784F852E72D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TeamsUsageStats" sheetId="1" r:id="rId1"/>
+    <sheet name="TeamsGroups" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
   <si>
     <t>uid</t>
   </si>
@@ -175,6 +176,60 @@
   </si>
   <si>
     <t>Actual Column Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single line of text </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GroupID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visibility </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CreatedOn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date and Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RenewedOn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeletedOn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ownerUID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">memberCount </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastActivity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">externalMemberCount </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modified </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created By </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Person or Group </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modified By </t>
   </si>
 </sst>
 </file>
@@ -541,8 +596,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,4 +884,189 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBB19B0-9638-42CA-B40A-DA0632514E11}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>